<commit_message>
FilmBewertung in AdminBereich hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumente/C#nema Zwischenstand.xlsx
+++ b/Dokumente/C#nema Zwischenstand.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>Programmieren 3 Projekt</t>
   </si>
@@ -629,12 +629,12 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="112" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
@@ -686,7 +686,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -749,7 +749,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -793,7 +793,10 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,7 +837,7 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
@@ -1103,7 +1106,10 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Dokumente (Zwischenstand, Änderungen) aktualisiert
</commit_message>
<xml_diff>
--- a/Dokumente/C#nema Zwischenstand.xlsx
+++ b/Dokumente/C#nema Zwischenstand.xlsx
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +725,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>

</xml_diff>